<commit_message>
Relación solicitud gráfica CN_10_10
Relación solicitud gráfica CN_10_10
</commit_message>
<xml_diff>
--- a/seguimiento/Grado10.xlsx
+++ b/seguimiento/Grado10.xlsx
@@ -840,7 +840,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,7 +1097,9 @@
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="E15" s="5">
+        <v>42222</v>
+      </c>
       <c r="F15" s="6"/>
       <c r="G15" s="10"/>
       <c r="H15" s="11"/>

</xml_diff>

<commit_message>
Relación solicitud grafica CN_10_11
Relación solicitud grafica CN_10_11
</commit_message>
<xml_diff>
--- a/seguimiento/Grado10.xlsx
+++ b/seguimiento/Grado10.xlsx
@@ -840,7 +840,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1115,9 @@
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="E16" s="5">
+        <v>42235</v>
+      </c>
       <c r="F16" s="6"/>
       <c r="G16" s="10"/>
       <c r="H16" s="11"/>

</xml_diff>